<commit_message>
add up to level 32
</commit_message>
<xml_diff>
--- a/levels/level10.xlsx
+++ b/levels/level10.xlsx
@@ -881,7 +881,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,7 +1009,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>1</v>

</xml_diff>